<commit_message>
Remove type_lieu from contrat modal
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,45 +423,89 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>mensuelle</v>
+        <v>444/AA4444</v>
       </c>
       <c r="B2" t="str">
         <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
-        <v>12345678</v>
+        <v>101</v>
       </c>
       <c r="D2" t="str">
-        <v>Youssef You</v>
+        <v>mmmmml</v>
       </c>
       <c r="E2" t="str">
         <v>ds</v>
       </c>
+      <c r="F2" t="str">
+        <v>mensuelle</v>
+      </c>
       <c r="G2">
-        <v>10000</v>
+        <v>12200</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>12200</v>
       </c>
       <c r="I2">
         <v>15</v>
       </c>
       <c r="J2">
+        <v>1830</v>
+      </c>
+      <c r="K2">
+        <v>1830</v>
+      </c>
+      <c r="L2">
+        <v>24400</v>
+      </c>
+      <c r="M2">
+        <v>10370</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>006/tESTDRR</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C3" t="str">
+        <v>aaaaa</v>
+      </c>
+      <c r="D3" t="str">
+        <v>aaaaaaa</v>
+      </c>
+      <c r="E3" t="str">
+        <v>ds</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>10000</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
+      </c>
+      <c r="J3">
         <v>1500</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="K3">
+        <v>1500</v>
+      </c>
+      <c r="L3">
+        <v>10000</v>
+      </c>
+      <c r="M3">
         <v>8500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add numero contrat generation function
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>797/DR TADLA</v>
+        <v>001/TEST DR</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>ad646456</v>
+        <v>BB779645</v>
       </c>
       <c r="D2" t="str">
-        <v>Mimo crimo</v>
+        <v>Karami abdelilah</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,33 +447,33 @@
         <v>--</v>
       </c>
       <c r="I2">
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="J2" t="str">
         <v>--</v>
       </c>
       <c r="K2">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="M2">
-        <v>5400</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>010/DR010/AV</v>
+        <v>001/TEST DR</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>aa654556</v>
+        <v>BG1949</v>
       </c>
       <c r="D3" t="str">
-        <v>Ali Ali</v>
+        <v>Ahmed Test</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -482,42 +482,42 @@
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H3" t="str">
         <v>--</v>
       </c>
       <c r="I3">
-        <v>2000</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>006/123</v>
+        <v>001/TEST DR</v>
       </c>
       <c r="B4" t="str">
-        <v>Siège</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>as46546</v>
+        <v>1196797</v>
       </c>
       <c r="D4" t="str">
-        <v>momi lomi</v>
+        <v>mediexpets</v>
       </c>
       <c r="E4" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F4" t="str">
         <v>mensuelle</v>
@@ -525,11 +525,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0</v>
+      <c r="H4" t="str">
+        <v>--</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -538,56 +538,138 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>001/TEST DR</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C5" t="str">
+        <v>BJ49785</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Anas tawfiqi</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>--</v>
+      </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>001/LF/TEST DR</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C6" t="str">
+        <v>1196797</v>
+      </c>
+      <c r="D6" t="str">
+        <v>mediexpets</v>
+      </c>
+      <c r="E6" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="str">
+        <v>--</v>
+      </c>
+      <c r="I6">
+        <v>90000</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>30000</v>
+      </c>
+      <c r="M6">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B5" t="str">
+      <c r="B7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C5" t="str">
+      <c r="C7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D5" t="str">
+      <c r="D7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E5" t="str">
+      <c r="E7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F5" t="str">
+      <c r="F7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G5" t="str">
+      <c r="G7" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>8000</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>600</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>7400</v>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>100000</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>800</v>
+      </c>
+      <c r="L7">
+        <v>40000</v>
+      </c>
+      <c r="M7">
+        <v>139200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix situation_cloture issue <contrat résilié>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>001/TEST DR</v>
+        <v>002/DR002/AV1</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>BB779645</v>
+        <v>BJ49785</v>
       </c>
       <c r="D2" t="str">
-        <v>Karami abdelilah</v>
+        <v>Anas tawfiqi</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -441,39 +441,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H2" t="str">
         <v>--</v>
       </c>
       <c r="I2">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="J2" t="str">
         <v>--</v>
       </c>
       <c r="K2">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="L2">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="M2">
-        <v>9500</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>001/TEST DR</v>
+        <v>002/DR002/AV1</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>BG1949</v>
+        <v>BB779645</v>
       </c>
       <c r="D3" t="str">
-        <v>Ahmed Test</v>
+        <v>Karami abdelilah</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -488,33 +488,33 @@
         <v>--</v>
       </c>
       <c r="I3">
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="J3" t="str">
         <v>--</v>
       </c>
       <c r="K3">
-        <v>300</v>
+        <v>750</v>
       </c>
       <c r="L3">
-        <v>3000</v>
+        <v>7500</v>
       </c>
       <c r="M3">
-        <v>5700</v>
+        <v>14250</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>001/TEST DR</v>
+        <v>108/ANSYSFYSN01/AV1</v>
       </c>
       <c r="B4" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>1196797</v>
+        <v>110384</v>
       </c>
       <c r="D4" t="str">
-        <v>mediexpets</v>
+        <v>real madrid fc</v>
       </c>
       <c r="E4" t="str">
         <v>oui</v>
@@ -525,11 +525,11 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" t="str">
-        <v>--</v>
+      <c r="H4">
+        <v>10000</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -538,24 +538,24 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>001/TEST DR</v>
+        <v>108/ANSYSFYSN01/AV1</v>
       </c>
       <c r="B5" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>BJ49785</v>
+        <v>KS10293</v>
       </c>
       <c r="D5" t="str">
-        <v>Anas tawfiqi</v>
+        <v>Karim benzima</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -564,42 +564,42 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <v>--</v>
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>3000</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>001/LF/TEST DR</v>
+        <v>108/ANSYSFYSN01/AV1</v>
       </c>
       <c r="B6" t="str">
-        <v>Logement de fonction</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C6" t="str">
-        <v>1196797</v>
+        <v>BB102938</v>
       </c>
       <c r="D6" t="str">
-        <v>mediexpets</v>
+        <v>Rodrigo silva jr</v>
       </c>
       <c r="E6" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F6" t="str">
         <v>mensuelle</v>
@@ -607,11 +607,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6" t="str">
-        <v>--</v>
+      <c r="H6">
+        <v>2000</v>
       </c>
       <c r="I6">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -620,24 +620,24 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>120000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>040/SUP SUD</v>
+        <v>108/ANSYSFYSN01/AV1</v>
       </c>
       <c r="B7" t="str">
-        <v>Supervision</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C7" t="str">
-        <v>BG1949</v>
+        <v>BJ119649</v>
       </c>
       <c r="D7" t="str">
-        <v>Ahmed Test</v>
+        <v>Test Test</v>
       </c>
       <c r="E7" t="str">
         <v>non</v>
@@ -646,25 +646,25 @@
         <v>mensuelle</v>
       </c>
       <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7" t="str">
-        <v>--</v>
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>4000</v>
       </c>
       <c r="I7">
-        <v>15000</v>
-      </c>
-      <c r="J7" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>400</v>
       </c>
       <c r="K7">
-        <v>2250</v>
+        <v>0</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>12750</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="8">
@@ -690,22 +690,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>19000</v>
       </c>
       <c r="I8">
-        <v>115000</v>
+        <v>17500</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="K8">
-        <v>3050</v>
+        <v>2250</v>
       </c>
       <c r="L8">
-        <v>40000</v>
+        <v>15000</v>
       </c>
       <c r="M8">
-        <v>151950</v>
+        <v>48550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix situation_cloture issue <contrat resilie> and update checkContratsAv function
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>002/DR002/AV1</v>
+        <v>794/DR KESH</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>BJ49785</v>
+        <v>BG1949</v>
       </c>
       <c r="D2" t="str">
-        <v>Anas tawfiqi</v>
+        <v>Ahmed Test</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -456,51 +456,51 @@
         <v>1500</v>
       </c>
       <c r="L2">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="M2">
-        <v>16000</v>
+        <v>8500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>002/DR002/AV1</v>
+        <v>108/ANSYSFYSN01/AV1</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>BB779645</v>
+        <v>110384</v>
       </c>
       <c r="D3" t="str">
-        <v>Karami abdelilah</v>
+        <v>real madrid fc</v>
       </c>
       <c r="E3" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F3" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>10000</v>
       </c>
       <c r="I3">
-        <v>7500</v>
-      </c>
-      <c r="J3" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>7500</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>14250</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="4">
@@ -511,28 +511,28 @@
         <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>110384</v>
+        <v>KS10293</v>
       </c>
       <c r="D4" t="str">
-        <v>real madrid fc</v>
+        <v>Karim benzima</v>
       </c>
       <c r="E4" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F4" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H4">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="M4">
-        <v>10000</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="5">
@@ -552,10 +552,10 @@
         <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>KS10293</v>
+        <v>BB102938</v>
       </c>
       <c r="D5" t="str">
-        <v>Karim benzima</v>
+        <v>Rodrigo silva jr</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -564,16 +564,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2700</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="6">
@@ -593,10 +593,10 @@
         <v>Direction régionale</v>
       </c>
       <c r="C6" t="str">
-        <v>BB102938</v>
+        <v>BJ119649</v>
       </c>
       <c r="D6" t="str">
-        <v>Rodrigo silva jr</v>
+        <v>Test Test</v>
       </c>
       <c r="E6" t="str">
         <v>non</v>
@@ -605,16 +605,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -623,94 +623,53 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>108/ANSYSFYSN01/AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B7" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C7" t="str">
-        <v>BJ119649</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D7" t="str">
-        <v>Test Test</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E7" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G7" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H7">
-        <v>4000</v>
+        <v>19000</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="J7">
-        <v>400</v>
+        <v>700</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M7">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G8" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H8">
-        <v>19000</v>
-      </c>
-      <c r="I8">
-        <v>17500</v>
-      </c>
-      <c r="J8">
-        <v>700</v>
-      </c>
-      <c r="K8">
-        <v>2250</v>
-      </c>
-      <c r="L8">
-        <v>15000</v>
-      </c>
-      <c r="M8">
-        <v>48550</v>
+        <v>26800</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Populate has_contrat with contrat <get all contrats>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,89 +423,89 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>794/DR KESH</v>
+        <v>108/ANSYSFYSN01</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>BG1949</v>
+        <v>110384</v>
       </c>
       <c r="D2" t="str">
-        <v>Ahmed Test</v>
+        <v>real madrid fc</v>
       </c>
       <c r="E2" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F2" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H2" t="str">
         <v>--</v>
       </c>
       <c r="I2">
-        <v>10000</v>
-      </c>
-      <c r="J2" t="str">
-        <v>--</v>
+        <v>9000</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>10000</v>
+        <v>3000</v>
       </c>
       <c r="M2">
-        <v>8500</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>108/ANSYSFYSN01/AV1</v>
+        <v>108/ANSYSFYSN01</v>
       </c>
       <c r="B3" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>110384</v>
+        <v>BB102938</v>
       </c>
       <c r="D3" t="str">
-        <v>real madrid fc</v>
+        <v>Rodrigo silva jr</v>
       </c>
       <c r="E3" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F3" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>10000</v>
+        <v>10</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
+        <v>18000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="M3">
-        <v>10000</v>
+        <v>22200</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>108/ANSYSFYSN01/AV1</v>
+        <v>108/ANSYSFYSN01</v>
       </c>
       <c r="B4" t="str">
         <v>Direction régionale</v>
@@ -523,153 +523,71 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
+      </c>
+      <c r="I4">
         <v>3000</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
       <c r="J4">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="M4">
-        <v>2700</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>108/ANSYSFYSN01/AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B5" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C5" t="str">
-        <v>BB102938</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D5" t="str">
-        <v>Rodrigo silva jr</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E5" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H5">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1800</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="M5">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>108/ANSYSFYSN01/AV1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C6" t="str">
-        <v>BJ119649</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Test Test</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>4000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>400</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H7">
-        <v>19000</v>
-      </c>
-      <c r="I7">
-        <v>10000</v>
-      </c>
-      <c r="J7">
-        <v>700</v>
-      </c>
-      <c r="K7">
-        <v>1500</v>
-      </c>
-      <c r="L7">
-        <v>10000</v>
-      </c>
-      <c r="M7">
-        <v>26800</v>
+        <v>38200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix situation cloture issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_5_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>001/TEST DR</v>
+        <v>001/WAFAE IMM</v>
       </c>
       <c r="B2" t="str">
-        <v>Direction régionale</v>
+        <v>Siège</v>
       </c>
       <c r="C2" t="str">
-        <v>BJ123456</v>
+        <v>HJ325474</v>
       </c>
       <c r="D2" t="str">
-        <v>TEST TEST</v>
+        <v>SOUMIA LALA</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -443,69 +443,438 @@
       <c r="G2">
         <v>15</v>
       </c>
-      <c r="H2">
-        <v>103547357.32</v>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>15532103.6</v>
+        <v>270000</v>
+      </c>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
-        <v>0</v>
+        <v>40500</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>88015253.73</v>
+        <v>229500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>887/TANGER MEDINA</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C3" t="str">
+        <v>HJ325474</v>
+      </c>
+      <c r="D3" t="str">
+        <v>SOUMIA LALA</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>annuelle</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>55879</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>5587.9</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>50291.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>887/TANGER MEDINA</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C4" t="str">
+        <v>68764654</v>
+      </c>
+      <c r="D4" t="str">
+        <v>STÉ LOCATION 22</v>
+      </c>
+      <c r="E4" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F4" t="str">
+        <v>annuelle</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>22336</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>22336</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>887/TANGER MEDINA</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C5" t="str">
+        <v>K3545445</v>
+      </c>
+      <c r="D5" t="str">
+        <v>HANANE TIFA</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>annuelle</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>21785</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>21785</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v xml:space="preserve">910/TANGER </v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>D235689</v>
+      </c>
+      <c r="D6" t="str">
+        <v>KAMILIA LALA</v>
+      </c>
+      <c r="E6" t="str">
+        <v>non</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6" t="str">
+        <v>--</v>
+      </c>
+      <c r="I6">
+        <v>24000</v>
+      </c>
+      <c r="J6" t="str">
+        <v>--</v>
+      </c>
+      <c r="K6">
+        <v>3600</v>
+      </c>
+      <c r="L6">
+        <v>24000</v>
+      </c>
+      <c r="M6">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v xml:space="preserve">910/TANGER </v>
+      </c>
+      <c r="B7" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Z213568</v>
+      </c>
+      <c r="D7" t="str">
+        <v>NABIL MOMO</v>
+      </c>
+      <c r="E7" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="str">
+        <v>--</v>
+      </c>
+      <c r="I7">
+        <v>16000</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>16000</v>
+      </c>
+      <c r="M7">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v xml:space="preserve">910/LF/TANGER </v>
+      </c>
+      <c r="B8" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C8" t="str">
+        <v>35464645</v>
+      </c>
+      <c r="D8" t="str">
+        <v>STÉ LOCATION 1</v>
+      </c>
+      <c r="E8" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>14161.71</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>14161.71</v>
+      </c>
+      <c r="M8">
+        <v>28323.43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v xml:space="preserve">910/LF/TANGER </v>
+      </c>
+      <c r="B9" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C9" t="str">
+        <v>L5245475</v>
+      </c>
+      <c r="D9" t="str">
+        <v>MORAD JOJO</v>
+      </c>
+      <c r="E9" t="str">
+        <v>non</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>5838.29</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>583.83</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>5838.29</v>
+      </c>
+      <c r="M9">
+        <v>11092.74</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>779/SUP TANGER 1</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C10" t="str">
+        <v>35464645</v>
+      </c>
+      <c r="D10" t="str">
+        <v>STÉ LOCATION 1</v>
+      </c>
+      <c r="E10" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F10" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>37500</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>75000</v>
+      </c>
+      <c r="M10">
+        <v>112500</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>779/SUP TANGER 1</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Z213568</v>
+      </c>
+      <c r="D11" t="str">
+        <v>NABIL MOMO</v>
+      </c>
+      <c r="E11" t="str">
+        <v>non</v>
+      </c>
+      <c r="F11" t="str">
+        <v>trimestrielle</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>12500</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1250</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>25000</v>
+      </c>
+      <c r="M11">
+        <v>36250</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B3" t="str">
+      <c r="B12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C3" t="str">
+      <c r="C12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D3" t="str">
+      <c r="D12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E3" t="str">
+      <c r="E12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F3" t="str">
+      <c r="F12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G3" t="str">
+      <c r="G12" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H3">
-        <v>103547357.32</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>15532103.6</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>88015253.73</v>
+      <c r="H12">
+        <v>170000</v>
+      </c>
+      <c r="I12">
+        <v>310000</v>
+      </c>
+      <c r="J12">
+        <v>7421.73</v>
+      </c>
+      <c r="K12">
+        <v>44100</v>
+      </c>
+      <c r="L12">
+        <v>160000</v>
+      </c>
+      <c r="M12">
+        <v>588478.27</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>